<commit_message>
detailed dem based clustering
</commit_message>
<xml_diff>
--- a/dimension-reduction/tones_encoded.xlsx
+++ b/dimension-reduction/tones_encoded.xlsx
@@ -436,162 +436,162 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>sample_1_Empathetic</t>
+          <t>sample_1_0</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>sample_1_Original</t>
+          <t>sample_1_1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>sample_1_Persuasive</t>
+          <t>sample_1_2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>sample_1_Simplier</t>
+          <t>sample_1_3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sample_2_Empathetic</t>
+          <t>sample_2_0</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>sample_2_Original</t>
+          <t>sample_2_1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sample_2_Persuasive</t>
+          <t>sample_2_2</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>sample_2_Simplier</t>
+          <t>sample_2_3</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>sample_3_Empathetic</t>
+          <t>sample_3_0</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>sample_3_Original</t>
+          <t>sample_3_1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>sample_3_Persuasive</t>
+          <t>sample_3_2</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>sample_3_Simplier</t>
+          <t>sample_3_3</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>sample_4_Empathetic</t>
+          <t>sample_4_0</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>sample_4_Original</t>
+          <t>sample_4_1</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>sample_4_Persuasive</t>
+          <t>sample_4_2</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>sample_4_Simplier</t>
+          <t>sample_4_3</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>sample_5_Empathetic</t>
+          <t>sample_5_0</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>sample_5_Original</t>
+          <t>sample_5_1</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>sample_5_Persuasive</t>
+          <t>sample_5_2</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>sample_5_Simplier</t>
+          <t>sample_5_3</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>sample_6_Empathetic</t>
+          <t>sample_6_0</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>sample_6_Original</t>
+          <t>sample_6_1</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>sample_6_Persuasive</t>
+          <t>sample_6_2</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>sample_6_Simplier</t>
+          <t>sample_6_3</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>sample_7_Empathetic</t>
+          <t>sample_7_0</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>sample_7_Original</t>
+          <t>sample_7_1</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>sample_7_Persuasive</t>
+          <t>sample_7_2</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>sample_7_Simplier</t>
+          <t>sample_7_3</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>sample_8_Empathetic</t>
+          <t>sample_8_0</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>sample_8_Original</t>
+          <t>sample_8_1</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>sample_8_Persuasive</t>
+          <t>sample_8_2</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>sample_8_Simplier</t>
+          <t>sample_8_3</t>
         </is>
       </c>
     </row>

</xml_diff>